<commit_message>
Ajustes na planilha de planejamento
</commit_message>
<xml_diff>
--- a/CHP/6.Gerenciamento de Projeto/Planejamento e Controle do Projeto.xlsx
+++ b/CHP/6.Gerenciamento de Projeto/Planejamento e Controle do Projeto.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Desktop\teste\chamado-pro\CHP\6.Gerenciamento de Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Equipe" sheetId="1" r:id="rId1"/>
@@ -6474,6 +6474,37 @@
     <xf numFmtId="164" fontId="39" fillId="3" borderId="1" xfId="16" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="164" fontId="40" fillId="3" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="169" fontId="40" fillId="9" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="170" fontId="40" fillId="9" borderId="1" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="41" fillId="3" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="170" fontId="40" fillId="11" borderId="1" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="40" fillId="3" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="171" fontId="40" fillId="9" borderId="1" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="171" fontId="40" fillId="11" borderId="1" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6481,18 +6512,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="3" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="3" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="4" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="6" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="16" fillId="7" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -6501,6 +6520,18 @@
     <xf numFmtId="164" fontId="13" fillId="5" borderId="2" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="3" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="3" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="4" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="6" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="22" fillId="5" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6518,21 +6549,6 @@
     </xf>
     <xf numFmtId="164" fontId="28" fillId="10" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="12" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="31" fillId="13" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="31" fillId="10" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="3" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="14" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="31" fillId="15" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -6548,6 +6564,21 @@
     <xf numFmtId="164" fontId="31" fillId="15" borderId="4" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="30" fillId="12" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="31" fillId="13" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="31" fillId="10" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="30" fillId="3" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="30" fillId="14" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="16" fillId="13" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6577,37 +6608,6 @@
     </xf>
     <xf numFmtId="164" fontId="29" fillId="6" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="40" fillId="3" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="169" fontId="40" fillId="9" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="170" fontId="40" fillId="9" borderId="1" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="41" fillId="3" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="170" fontId="40" fillId="11" borderId="1" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="40" fillId="3" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="171" fontId="40" fillId="9" borderId="1" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="171" fontId="40" fillId="11" borderId="1" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="17">
@@ -8490,7 +8490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -8504,18 +8504,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="123" t="s">
+      <c r="A1" s="131" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="123"/>
-      <c r="C1" s="123"/>
+      <c r="B1" s="131"/>
+      <c r="C1" s="131"/>
     </row>
     <row r="2" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="124" t="s">
+      <c r="A2" s="132" t="s">
         <v>220</v>
       </c>
-      <c r="B2" s="124"/>
-      <c r="C2" s="124"/>
+      <c r="B2" s="132"/>
+      <c r="C2" s="132"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -8651,8 +8651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ46"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29:D32"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8672,38 +8672,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="131" t="s">
+      <c r="A1" s="135" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="131"/>
-      <c r="C1" s="131"/>
-      <c r="D1" s="131"/>
-      <c r="F1" s="125" t="s">
+      <c r="B1" s="135"/>
+      <c r="C1" s="135"/>
+      <c r="D1" s="135"/>
+      <c r="F1" s="136" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="125"/>
-      <c r="H1" s="125"/>
-      <c r="I1" s="125"/>
-      <c r="J1" s="125"/>
-      <c r="K1" s="125"/>
-      <c r="L1" s="125"/>
+      <c r="G1" s="136"/>
+      <c r="H1" s="136"/>
+      <c r="I1" s="136"/>
+      <c r="J1" s="136"/>
+      <c r="K1" s="136"/>
+      <c r="L1" s="136"/>
     </row>
     <row r="2" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="126" t="s">
+      <c r="A2" s="137" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="126"/>
-      <c r="C2" s="126"/>
-      <c r="D2" s="126"/>
-      <c r="F2" s="127" t="s">
+      <c r="B2" s="137"/>
+      <c r="C2" s="137"/>
+      <c r="D2" s="137"/>
+      <c r="F2" s="138" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="127"/>
-      <c r="H2" s="127"/>
-      <c r="I2" s="127"/>
-      <c r="J2" s="127"/>
-      <c r="K2" s="127"/>
-      <c r="L2" s="127"/>
+      <c r="G2" s="138"/>
+      <c r="H2" s="138"/>
+      <c r="I2" s="138"/>
+      <c r="J2" s="138"/>
+      <c r="K2" s="138"/>
+      <c r="L2" s="138"/>
     </row>
     <row r="3" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
@@ -8724,20 +8724,20 @@
       <c r="G3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="128" t="s">
+      <c r="H3" s="139" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="128"/>
-      <c r="J3" s="128"/>
-      <c r="K3" s="128"/>
-      <c r="L3" s="128"/>
+      <c r="I3" s="139"/>
+      <c r="J3" s="139"/>
+      <c r="K3" s="139"/>
+      <c r="L3" s="139"/>
     </row>
     <row r="4" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="129" t="s">
+      <c r="A4" s="133" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="129"/>
-      <c r="C4" s="129"/>
+      <c r="B4" s="133"/>
+      <c r="C4" s="133"/>
       <c r="D4" s="8" t="s">
         <v>17</v>
       </c>
@@ -8970,11 +8970,11 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="129" t="s">
+      <c r="A11" s="133" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="129"/>
-      <c r="C11" s="129"/>
+      <c r="B11" s="133"/>
+      <c r="C11" s="133"/>
       <c r="D11" s="8">
         <f>SUM(D5:D10)</f>
         <v>24</v>
@@ -9077,7 +9077,7 @@
         <v>232</v>
       </c>
       <c r="D15" s="13">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F15" s="17"/>
       <c r="G15" s="12"/>
@@ -9101,7 +9101,7 @@
         <v>35</v>
       </c>
       <c r="D16" s="13">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F16" s="17"/>
       <c r="G16" s="12"/>
@@ -9149,7 +9149,7 @@
         <v>37</v>
       </c>
       <c r="D18" s="13">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F18" s="17"/>
       <c r="G18" s="12"/>
@@ -9201,14 +9201,14 @@
       <c r="L20" s="21"/>
     </row>
     <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="129" t="s">
+      <c r="A21" s="133" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="129"/>
-      <c r="C21" s="129"/>
+      <c r="B21" s="133"/>
+      <c r="C21" s="133"/>
       <c r="D21" s="8">
         <f>SUM(D12:D20)</f>
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="H21" s="21"/>
       <c r="I21" s="21"/>
@@ -9404,11 +9404,11 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="129" t="s">
+      <c r="A35" s="133" t="s">
         <v>41</v>
       </c>
-      <c r="B35" s="129"/>
-      <c r="C35" s="129"/>
+      <c r="B35" s="133"/>
+      <c r="C35" s="133"/>
       <c r="D35" s="8">
         <f>SUM(D22:D34)</f>
         <v>102</v>
@@ -9541,9 +9541,9 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="130"/>
-      <c r="B45" s="130"/>
-      <c r="C45" s="130"/>
+      <c r="A45" s="134"/>
+      <c r="B45" s="134"/>
+      <c r="C45" s="134"/>
       <c r="D45" s="8">
         <f>SUM(D36:D44)</f>
         <v>28</v>
@@ -9552,21 +9552,21 @@
     <row r="46" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="D46" s="24">
         <f>SUM(D11,D21,D35,D45)</f>
-        <v>198</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="F1:L1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="F2:L2"/>
+    <mergeCell ref="H3:L3"/>
+    <mergeCell ref="A4:C4"/>
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="A21:C21"/>
     <mergeCell ref="A35:C35"/>
     <mergeCell ref="A45:C45"/>
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="F1:L1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="F2:L2"/>
-    <mergeCell ref="H3:L3"/>
-    <mergeCell ref="A4:C4"/>
   </mergeCells>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="1.1437007874015752" bottom="1.1437007874015752" header="0.75000000000000011" footer="0.75000000000000011"/>
   <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -9594,19 +9594,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="132" t="s">
+      <c r="A1" s="140" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="132"/>
-      <c r="C1" s="132"/>
+      <c r="B1" s="140"/>
+      <c r="C1" s="140"/>
     </row>
     <row r="2" spans="1:5" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="133" t="s">
+      <c r="A3" s="141" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="133"/>
-      <c r="C3" s="133"/>
+      <c r="B3" s="141"/>
+      <c r="C3" s="141"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
@@ -9614,7 +9614,7 @@
       </c>
       <c r="B4" s="27">
         <f>Backlog_Produto!$D$46</f>
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="C4" s="26" t="s">
         <v>52</v>
@@ -9672,7 +9672,7 @@
       </c>
       <c r="B9" s="34">
         <f>B11/2</f>
-        <v>2.97</v>
+        <v>3.03</v>
       </c>
       <c r="C9" s="33" t="s">
         <v>60</v>
@@ -9684,7 +9684,7 @@
       </c>
       <c r="B10" s="34">
         <f>B4+(B4*B5)</f>
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="C10" s="35" t="s">
         <v>52</v>
@@ -9696,7 +9696,7 @@
       </c>
       <c r="B11" s="32">
         <f>B10/B8*2</f>
-        <v>5.94</v>
+        <v>6.06</v>
       </c>
       <c r="C11" s="30" t="s">
         <v>63</v>
@@ -9708,18 +9708,18 @@
       </c>
       <c r="B12" s="36">
         <f>B11/4</f>
-        <v>1.4850000000000001</v>
+        <v>1.5149999999999999</v>
       </c>
       <c r="C12" s="26" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="133" t="s">
+      <c r="A14" s="141" t="s">
         <v>66</v>
       </c>
-      <c r="B14" s="133"/>
-      <c r="C14" s="133"/>
+      <c r="B14" s="141"/>
+      <c r="C14" s="141"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="30" t="s">
@@ -9736,7 +9736,7 @@
       </c>
       <c r="B16" s="39">
         <f>B10*B15</f>
-        <v>5940</v>
+        <v>6060</v>
       </c>
       <c r="C16" s="38"/>
     </row>
@@ -9755,7 +9755,7 @@
       </c>
       <c r="B18" s="40">
         <f>B16*B17</f>
-        <v>1188</v>
+        <v>1212</v>
       </c>
       <c r="C18" s="38"/>
     </row>
@@ -9765,7 +9765,7 @@
       </c>
       <c r="B19" s="42">
         <f>B16+B18</f>
-        <v>7128</v>
+        <v>7272</v>
       </c>
       <c r="C19" s="38"/>
     </row>
@@ -9784,7 +9784,7 @@
       </c>
       <c r="B21" s="43">
         <f>B19*B20</f>
-        <v>1425.6000000000001</v>
+        <v>1454.4</v>
       </c>
       <c r="C21" s="38"/>
     </row>
@@ -9794,7 +9794,7 @@
       </c>
       <c r="B22" s="42">
         <f>B19+B21</f>
-        <v>8553.6</v>
+        <v>8726.4</v>
       </c>
       <c r="C22" s="38"/>
     </row>
@@ -9833,54 +9833,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="134" t="s">
+      <c r="A1" s="142" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="134"/>
-      <c r="C1" s="134"/>
-      <c r="D1" s="134"/>
-      <c r="E1" s="134"/>
-      <c r="F1" s="134"/>
-      <c r="G1" s="134"/>
-      <c r="H1" s="134"/>
-      <c r="I1" s="134"/>
-      <c r="J1" s="134"/>
-      <c r="K1" s="134"/>
+      <c r="B1" s="142"/>
+      <c r="C1" s="142"/>
+      <c r="D1" s="142"/>
+      <c r="E1" s="142"/>
+      <c r="F1" s="142"/>
+      <c r="G1" s="142"/>
+      <c r="H1" s="142"/>
+      <c r="I1" s="142"/>
+      <c r="J1" s="142"/>
+      <c r="K1" s="142"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="135" t="s">
+      <c r="A2" s="143" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="135"/>
-      <c r="C2" s="135"/>
-      <c r="D2" s="135"/>
+      <c r="B2" s="143"/>
+      <c r="C2" s="143"/>
+      <c r="D2" s="143"/>
       <c r="E2" s="44">
         <f>Planejamento!$B$10</f>
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="F2" s="45"/>
-      <c r="G2" s="135" t="s">
+      <c r="G2" s="143" t="s">
         <v>76</v>
       </c>
-      <c r="H2" s="135"/>
-      <c r="I2" s="135"/>
-      <c r="J2" s="135"/>
+      <c r="H2" s="143"/>
+      <c r="I2" s="143"/>
+      <c r="J2" s="143"/>
       <c r="K2" s="44"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="46"/>
       <c r="B3" s="47"/>
-      <c r="C3" s="136" t="s">
+      <c r="C3" s="144" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="136"/>
-      <c r="E3" s="136"/>
+      <c r="D3" s="144"/>
+      <c r="E3" s="144"/>
       <c r="F3" s="48"/>
-      <c r="G3" s="137" t="s">
+      <c r="G3" s="145" t="s">
         <v>78</v>
       </c>
-      <c r="H3" s="137"/>
-      <c r="I3" s="137"/>
+      <c r="H3" s="145"/>
+      <c r="I3" s="145"/>
       <c r="J3" s="50"/>
       <c r="K3" s="51"/>
     </row>
@@ -9923,35 +9923,35 @@
       <c r="A5" s="53">
         <v>1</v>
       </c>
-      <c r="B5" s="159" t="s">
+      <c r="B5" s="123" t="s">
         <v>87</v>
       </c>
-      <c r="C5" s="160">
+      <c r="C5" s="124">
         <v>45894</v>
       </c>
-      <c r="D5" s="160">
+      <c r="D5" s="124">
         <v>45903</v>
       </c>
-      <c r="E5" s="161">
+      <c r="E5" s="125">
         <v>24</v>
       </c>
-      <c r="F5" s="162" t="s">
+      <c r="F5" s="126" t="s">
         <v>88</v>
       </c>
-      <c r="G5" s="160">
+      <c r="G5" s="124">
         <v>43132</v>
       </c>
-      <c r="H5" s="160">
+      <c r="H5" s="124">
         <v>43160</v>
       </c>
-      <c r="I5" s="161">
+      <c r="I5" s="125">
         <v>28</v>
       </c>
-      <c r="J5" s="163">
+      <c r="J5" s="127">
         <f>E5-I5</f>
         <v>-4</v>
       </c>
-      <c r="K5" s="164" t="s">
+      <c r="K5" s="128" t="s">
         <v>89</v>
       </c>
     </row>
@@ -9959,51 +9959,51 @@
       <c r="A6" s="53">
         <v>2</v>
       </c>
-      <c r="B6" s="159" t="s">
+      <c r="B6" s="123" t="s">
         <v>249</v>
       </c>
-      <c r="C6" s="160">
+      <c r="C6" s="124">
         <v>45904</v>
       </c>
-      <c r="D6" s="160">
+      <c r="D6" s="124">
         <v>45931</v>
       </c>
-      <c r="E6" s="165">
+      <c r="E6" s="129">
         <v>36</v>
       </c>
-      <c r="F6" s="162" t="s">
+      <c r="F6" s="126" t="s">
         <v>90</v>
       </c>
-      <c r="G6" s="160"/>
-      <c r="H6" s="160"/>
-      <c r="I6" s="165"/>
-      <c r="J6" s="166"/>
-      <c r="K6" s="164"/>
+      <c r="G6" s="124"/>
+      <c r="H6" s="124"/>
+      <c r="I6" s="129"/>
+      <c r="J6" s="130"/>
+      <c r="K6" s="128"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="53">
         <v>3</v>
       </c>
-      <c r="B7" s="159" t="s">
+      <c r="B7" s="123" t="s">
         <v>248</v>
       </c>
-      <c r="C7" s="160">
+      <c r="C7" s="124">
         <v>45932</v>
       </c>
-      <c r="D7" s="160">
+      <c r="D7" s="124">
         <v>45951</v>
       </c>
-      <c r="E7" s="161">
+      <c r="E7" s="125">
         <v>24</v>
       </c>
-      <c r="F7" s="162" t="s">
+      <c r="F7" s="126" t="s">
         <v>90</v>
       </c>
-      <c r="G7" s="160"/>
-      <c r="H7" s="160"/>
-      <c r="I7" s="165"/>
-      <c r="J7" s="166"/>
-      <c r="K7" s="164"/>
+      <c r="G7" s="124"/>
+      <c r="H7" s="124"/>
+      <c r="I7" s="129"/>
+      <c r="J7" s="130"/>
+      <c r="K7" s="128"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="53">
@@ -10021,7 +10021,7 @@
       <c r="E8" s="56">
         <v>34</v>
       </c>
-      <c r="F8" s="162" t="s">
+      <c r="F8" s="126" t="s">
         <v>90</v>
       </c>
       <c r="G8" s="55"/>
@@ -10257,19 +10257,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="67" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="134" t="s">
+      <c r="A1" s="142" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="134"/>
-      <c r="C1" s="134"/>
-      <c r="D1" s="134"/>
-      <c r="E1" s="134"/>
-      <c r="F1" s="134"/>
-      <c r="G1" s="134"/>
-      <c r="H1" s="134"/>
-      <c r="I1" s="134"/>
-      <c r="J1" s="134"/>
-      <c r="K1" s="134"/>
+      <c r="B1" s="142"/>
+      <c r="C1" s="142"/>
+      <c r="D1" s="142"/>
+      <c r="E1" s="142"/>
+      <c r="F1" s="142"/>
+      <c r="G1" s="142"/>
+      <c r="H1" s="142"/>
+      <c r="I1" s="142"/>
+      <c r="J1" s="142"/>
+      <c r="K1" s="142"/>
     </row>
     <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
@@ -10423,10 +10423,10 @@
       </c>
     </row>
     <row r="33" spans="1:11" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D33" s="139" t="s">
+      <c r="D33" s="153" t="s">
         <v>122</v>
       </c>
-      <c r="E33" s="139"/>
+      <c r="E33" s="153"/>
     </row>
     <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="D34" s="70">
@@ -10478,137 +10478,137 @@
     </row>
     <row r="40" spans="1:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="41" spans="1:11" s="67" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="140" t="s">
+      <c r="A41" s="154" t="s">
         <v>129</v>
       </c>
-      <c r="B41" s="140"/>
-      <c r="C41" s="140"/>
-      <c r="D41" s="140"/>
-      <c r="E41" s="140"/>
-      <c r="F41" s="140"/>
-      <c r="G41" s="140"/>
-      <c r="H41" s="140"/>
-      <c r="I41" s="140"/>
-      <c r="J41" s="140"/>
-      <c r="K41" s="140"/>
+      <c r="B41" s="154"/>
+      <c r="C41" s="154"/>
+      <c r="D41" s="154"/>
+      <c r="E41" s="154"/>
+      <c r="F41" s="154"/>
+      <c r="G41" s="154"/>
+      <c r="H41" s="154"/>
+      <c r="I41" s="154"/>
+      <c r="J41" s="154"/>
+      <c r="K41" s="154"/>
     </row>
     <row r="42" spans="1:11" s="67" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="141" t="s">
+      <c r="A42" s="155" t="s">
         <v>130</v>
       </c>
-      <c r="B42" s="141"/>
-      <c r="C42" s="141"/>
-      <c r="D42" s="141"/>
-      <c r="E42" s="141"/>
-      <c r="F42" s="141"/>
-      <c r="G42" s="141"/>
-      <c r="H42" s="141"/>
-      <c r="I42" s="141"/>
-      <c r="J42" s="141"/>
-      <c r="K42" s="141"/>
+      <c r="B42" s="155"/>
+      <c r="C42" s="155"/>
+      <c r="D42" s="155"/>
+      <c r="E42" s="155"/>
+      <c r="F42" s="155"/>
+      <c r="G42" s="155"/>
+      <c r="H42" s="155"/>
+      <c r="I42" s="155"/>
+      <c r="J42" s="155"/>
+      <c r="K42" s="155"/>
     </row>
     <row r="43" spans="1:11" s="67" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="142" t="s">
+      <c r="A43" s="156" t="s">
         <v>131</v>
       </c>
-      <c r="B43" s="142"/>
-      <c r="C43" s="142"/>
-      <c r="D43" s="142"/>
-      <c r="E43" s="142"/>
-      <c r="F43" s="142"/>
-      <c r="G43" s="142"/>
-      <c r="H43" s="142"/>
-      <c r="I43" s="142"/>
-      <c r="J43" s="142"/>
-      <c r="K43" s="142"/>
+      <c r="B43" s="156"/>
+      <c r="C43" s="156"/>
+      <c r="D43" s="156"/>
+      <c r="E43" s="156"/>
+      <c r="F43" s="156"/>
+      <c r="G43" s="156"/>
+      <c r="H43" s="156"/>
+      <c r="I43" s="156"/>
+      <c r="J43" s="156"/>
+      <c r="K43" s="156"/>
     </row>
     <row r="44" spans="1:11" s="67" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="138" t="s">
+      <c r="A44" s="152" t="s">
         <v>132</v>
       </c>
-      <c r="B44" s="138"/>
-      <c r="C44" s="138"/>
-      <c r="D44" s="138"/>
-      <c r="E44" s="138"/>
-      <c r="F44" s="138"/>
-      <c r="G44" s="138"/>
-      <c r="H44" s="138"/>
-      <c r="I44" s="138"/>
-      <c r="J44" s="138"/>
-      <c r="K44" s="138"/>
+      <c r="B44" s="152"/>
+      <c r="C44" s="152"/>
+      <c r="D44" s="152"/>
+      <c r="E44" s="152"/>
+      <c r="F44" s="152"/>
+      <c r="G44" s="152"/>
+      <c r="H44" s="152"/>
+      <c r="I44" s="152"/>
+      <c r="J44" s="152"/>
+      <c r="K44" s="152"/>
     </row>
     <row r="45" spans="1:11" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="46" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="145" t="s">
+      <c r="A46" s="148" t="s">
         <v>133</v>
       </c>
-      <c r="B46" s="145"/>
-      <c r="C46" s="145"/>
-      <c r="D46" s="145"/>
-      <c r="E46" s="145"/>
-      <c r="F46" s="145"/>
-      <c r="G46" s="145"/>
-      <c r="H46" s="145"/>
-      <c r="I46" s="145"/>
-      <c r="J46" s="145"/>
-      <c r="K46" s="145"/>
+      <c r="B46" s="148"/>
+      <c r="C46" s="148"/>
+      <c r="D46" s="148"/>
+      <c r="E46" s="148"/>
+      <c r="F46" s="148"/>
+      <c r="G46" s="148"/>
+      <c r="H46" s="148"/>
+      <c r="I46" s="148"/>
+      <c r="J46" s="148"/>
+      <c r="K46" s="148"/>
     </row>
     <row r="47" spans="1:11" s="76" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="74" t="s">
         <v>134</v>
       </c>
       <c r="B47" s="75"/>
-      <c r="C47" s="146" t="s">
+      <c r="C47" s="149" t="s">
         <v>135</v>
       </c>
-      <c r="D47" s="146"/>
-      <c r="E47" s="146"/>
-      <c r="F47" s="146"/>
-      <c r="G47" s="146"/>
-      <c r="H47" s="146"/>
-      <c r="I47" s="146"/>
-      <c r="J47" s="146"/>
-      <c r="K47" s="146"/>
+      <c r="D47" s="149"/>
+      <c r="E47" s="149"/>
+      <c r="F47" s="149"/>
+      <c r="G47" s="149"/>
+      <c r="H47" s="149"/>
+      <c r="I47" s="149"/>
+      <c r="J47" s="149"/>
+      <c r="K47" s="149"/>
     </row>
     <row r="48" spans="1:11" s="78" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="147"/>
-      <c r="B48" s="143" t="s">
+      <c r="A48" s="150"/>
+      <c r="B48" s="146" t="s">
         <v>136</v>
       </c>
-      <c r="C48" s="143" t="s">
+      <c r="C48" s="146" t="s">
         <v>137</v>
       </c>
-      <c r="D48" s="143" t="s">
+      <c r="D48" s="146" t="s">
         <v>138</v>
       </c>
-      <c r="E48" s="143" t="s">
+      <c r="E48" s="146" t="s">
         <v>107</v>
       </c>
-      <c r="F48" s="143" t="s">
+      <c r="F48" s="146" t="s">
         <v>139</v>
       </c>
-      <c r="G48" s="143" t="s">
+      <c r="G48" s="146" t="s">
         <v>111</v>
       </c>
-      <c r="H48" s="148" t="s">
+      <c r="H48" s="151" t="s">
         <v>140</v>
       </c>
-      <c r="I48" s="148"/>
-      <c r="J48" s="148"/>
-      <c r="K48" s="148"/>
+      <c r="I48" s="151"/>
+      <c r="J48" s="151"/>
+      <c r="K48" s="151"/>
     </row>
     <row r="49" spans="1:11" s="78" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="147"/>
-      <c r="B49" s="143"/>
-      <c r="C49" s="143"/>
-      <c r="D49" s="143"/>
-      <c r="E49" s="143"/>
-      <c r="F49" s="143"/>
-      <c r="G49" s="143"/>
-      <c r="H49" s="143" t="s">
+      <c r="A49" s="150"/>
+      <c r="B49" s="146"/>
+      <c r="C49" s="146"/>
+      <c r="D49" s="146"/>
+      <c r="E49" s="146"/>
+      <c r="F49" s="146"/>
+      <c r="G49" s="146"/>
+      <c r="H49" s="146" t="s">
         <v>141</v>
       </c>
-      <c r="I49" s="143"/>
+      <c r="I49" s="146"/>
       <c r="J49" s="77" t="s">
         <v>142</v>
       </c>
@@ -10639,8 +10639,8 @@
       <c r="G50" s="82" t="s">
         <v>112</v>
       </c>
-      <c r="H50" s="144"/>
-      <c r="I50" s="144"/>
+      <c r="H50" s="147"/>
+      <c r="I50" s="147"/>
       <c r="J50" s="84"/>
       <c r="K50" s="84" t="s">
         <v>145</v>
@@ -10787,8 +10787,8 @@
         <v>#VALUE!</v>
       </c>
       <c r="G59" s="82"/>
-      <c r="H59" s="144"/>
-      <c r="I59" s="144"/>
+      <c r="H59" s="147"/>
+      <c r="I59" s="147"/>
       <c r="J59" s="84"/>
       <c r="K59" s="84"/>
     </row>
@@ -10803,13 +10803,19 @@
         <v>#VALUE!</v>
       </c>
       <c r="G60" s="82"/>
-      <c r="H60" s="144"/>
-      <c r="I60" s="144"/>
+      <c r="H60" s="147"/>
+      <c r="I60" s="147"/>
       <c r="J60" s="84"/>
       <c r="K60" s="84"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A44:K44"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="A41:K41"/>
+    <mergeCell ref="A42:K42"/>
+    <mergeCell ref="A43:K43"/>
     <mergeCell ref="H49:I49"/>
     <mergeCell ref="H50:I50"/>
     <mergeCell ref="H59:I59"/>
@@ -10824,12 +10830,6 @@
     <mergeCell ref="F48:F49"/>
     <mergeCell ref="G48:G49"/>
     <mergeCell ref="H48:K48"/>
-    <mergeCell ref="A44:K44"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="A41:K41"/>
-    <mergeCell ref="A42:K42"/>
-    <mergeCell ref="A43:K43"/>
   </mergeCells>
   <conditionalFormatting sqref="F50:F60">
     <cfRule type="cellIs" dxfId="2" priority="8" stopIfTrue="1" operator="equal">
@@ -10892,116 +10892,116 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="67" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="151" t="s">
+      <c r="A1" s="159" t="s">
         <v>146</v>
       </c>
-      <c r="B1" s="151"/>
-      <c r="C1" s="151"/>
-      <c r="D1" s="151"/>
-      <c r="E1" s="151"/>
-      <c r="F1" s="151"/>
-      <c r="G1" s="151"/>
-      <c r="H1" s="151"/>
-      <c r="I1" s="151"/>
-      <c r="J1" s="151"/>
-      <c r="K1" s="151"/>
-      <c r="L1" s="151"/>
-      <c r="M1" s="151"/>
-      <c r="N1" s="151"/>
+      <c r="B1" s="159"/>
+      <c r="C1" s="159"/>
+      <c r="D1" s="159"/>
+      <c r="E1" s="159"/>
+      <c r="F1" s="159"/>
+      <c r="G1" s="159"/>
+      <c r="H1" s="159"/>
+      <c r="I1" s="159"/>
+      <c r="J1" s="159"/>
+      <c r="K1" s="159"/>
+      <c r="L1" s="159"/>
+      <c r="M1" s="159"/>
+      <c r="N1" s="159"/>
     </row>
     <row r="2" spans="1:23" s="87" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="152" t="s">
+      <c r="A2" s="160" t="s">
         <v>129</v>
       </c>
-      <c r="B2" s="152"/>
-      <c r="C2" s="152"/>
-      <c r="D2" s="152"/>
-      <c r="E2" s="152"/>
-      <c r="F2" s="152"/>
-      <c r="G2" s="152"/>
-      <c r="H2" s="152"/>
-      <c r="I2" s="152"/>
-      <c r="J2" s="152"/>
-      <c r="K2" s="152"/>
-      <c r="L2" s="152"/>
-      <c r="M2" s="152"/>
-      <c r="N2" s="152"/>
+      <c r="B2" s="160"/>
+      <c r="C2" s="160"/>
+      <c r="D2" s="160"/>
+      <c r="E2" s="160"/>
+      <c r="F2" s="160"/>
+      <c r="G2" s="160"/>
+      <c r="H2" s="160"/>
+      <c r="I2" s="160"/>
+      <c r="J2" s="160"/>
+      <c r="K2" s="160"/>
+      <c r="L2" s="160"/>
+      <c r="M2" s="160"/>
+      <c r="N2" s="160"/>
     </row>
     <row r="3" spans="1:23" s="87" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="153" t="s">
+      <c r="A3" s="161" t="s">
         <v>147</v>
       </c>
-      <c r="B3" s="153"/>
-      <c r="C3" s="153"/>
-      <c r="D3" s="153"/>
-      <c r="E3" s="153"/>
-      <c r="F3" s="153"/>
-      <c r="G3" s="153"/>
-      <c r="H3" s="153"/>
-      <c r="I3" s="153"/>
-      <c r="J3" s="153"/>
-      <c r="K3" s="153"/>
-      <c r="L3" s="153"/>
-      <c r="M3" s="153"/>
-      <c r="N3" s="153"/>
+      <c r="B3" s="161"/>
+      <c r="C3" s="161"/>
+      <c r="D3" s="161"/>
+      <c r="E3" s="161"/>
+      <c r="F3" s="161"/>
+      <c r="G3" s="161"/>
+      <c r="H3" s="161"/>
+      <c r="I3" s="161"/>
+      <c r="J3" s="161"/>
+      <c r="K3" s="161"/>
+      <c r="L3" s="161"/>
+      <c r="M3" s="161"/>
+      <c r="N3" s="161"/>
     </row>
     <row r="4" spans="1:23" s="87" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="154" t="s">
+      <c r="A4" s="162" t="s">
         <v>148</v>
       </c>
-      <c r="B4" s="154"/>
-      <c r="C4" s="154"/>
-      <c r="D4" s="154"/>
-      <c r="E4" s="154"/>
-      <c r="F4" s="154"/>
-      <c r="G4" s="154"/>
-      <c r="H4" s="154"/>
-      <c r="I4" s="154"/>
-      <c r="J4" s="154"/>
-      <c r="K4" s="154"/>
-      <c r="L4" s="154"/>
-      <c r="M4" s="154"/>
-      <c r="N4" s="154"/>
+      <c r="B4" s="162"/>
+      <c r="C4" s="162"/>
+      <c r="D4" s="162"/>
+      <c r="E4" s="162"/>
+      <c r="F4" s="162"/>
+      <c r="G4" s="162"/>
+      <c r="H4" s="162"/>
+      <c r="I4" s="162"/>
+      <c r="J4" s="162"/>
+      <c r="K4" s="162"/>
+      <c r="L4" s="162"/>
+      <c r="M4" s="162"/>
+      <c r="N4" s="162"/>
     </row>
     <row r="5" spans="1:23" s="87" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="155" t="s">
+      <c r="A5" s="163" t="s">
         <v>149</v>
       </c>
-      <c r="B5" s="155"/>
-      <c r="C5" s="155"/>
-      <c r="D5" s="155"/>
-      <c r="E5" s="155"/>
-      <c r="F5" s="155"/>
-      <c r="G5" s="155"/>
-      <c r="H5" s="155"/>
-      <c r="I5" s="155"/>
-      <c r="J5" s="155"/>
-      <c r="K5" s="155"/>
-      <c r="L5" s="155"/>
-      <c r="M5" s="155"/>
-      <c r="N5" s="155"/>
+      <c r="B5" s="163"/>
+      <c r="C5" s="163"/>
+      <c r="D5" s="163"/>
+      <c r="E5" s="163"/>
+      <c r="F5" s="163"/>
+      <c r="G5" s="163"/>
+      <c r="H5" s="163"/>
+      <c r="I5" s="163"/>
+      <c r="J5" s="163"/>
+      <c r="K5" s="163"/>
+      <c r="L5" s="163"/>
+      <c r="M5" s="163"/>
+      <c r="N5" s="163"/>
     </row>
     <row r="6" spans="1:23" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:23" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="149" t="s">
+      <c r="A7" s="157" t="s">
         <v>150</v>
       </c>
-      <c r="B7" s="149"/>
-      <c r="D7" s="149" t="s">
+      <c r="B7" s="157"/>
+      <c r="D7" s="157" t="s">
         <v>151</v>
       </c>
-      <c r="E7" s="149"/>
-      <c r="G7" s="149" t="s">
+      <c r="E7" s="157"/>
+      <c r="G7" s="157" t="s">
         <v>152</v>
       </c>
-      <c r="H7" s="149"/>
-      <c r="I7" s="149"/>
-      <c r="J7" s="149"/>
-      <c r="K7" s="149"/>
-      <c r="M7" s="149" t="s">
+      <c r="H7" s="157"/>
+      <c r="I7" s="157"/>
+      <c r="J7" s="157"/>
+      <c r="K7" s="157"/>
+      <c r="M7" s="157" t="s">
         <v>153</v>
       </c>
-      <c r="N7" s="149"/>
+      <c r="N7" s="157"/>
     </row>
     <row r="8" spans="1:23" s="4" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="90" t="s">
@@ -11101,13 +11101,13 @@
       <c r="B11" s="89"/>
       <c r="D11" s="88"/>
       <c r="E11" s="89"/>
-      <c r="G11" s="149" t="s">
+      <c r="G11" s="157" t="s">
         <v>170</v>
       </c>
-      <c r="H11" s="149"/>
-      <c r="I11" s="149"/>
-      <c r="J11" s="149"/>
-      <c r="K11" s="149"/>
+      <c r="H11" s="157"/>
+      <c r="I11" s="157"/>
+      <c r="J11" s="157"/>
+      <c r="K11" s="157"/>
       <c r="M11" s="92" t="s">
         <v>171</v>
       </c>
@@ -11210,12 +11210,12 @@
       <c r="B16" s="89"/>
       <c r="D16" s="88"/>
       <c r="E16" s="89"/>
-      <c r="G16" s="150" t="s">
+      <c r="G16" s="158" t="s">
         <v>180</v>
       </c>
-      <c r="H16" s="150"/>
-      <c r="I16" s="150"/>
-      <c r="J16" s="150"/>
+      <c r="H16" s="158"/>
+      <c r="I16" s="158"/>
+      <c r="J16" s="158"/>
       <c r="K16" s="94">
         <f>SUM(K9,K10,K13,K14,K15)</f>
         <v>14</v>
@@ -11380,42 +11380,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="151" t="s">
+      <c r="A1" s="159" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="151"/>
-      <c r="C1" s="151"/>
-      <c r="D1" s="151"/>
-      <c r="E1" s="151"/>
-      <c r="F1" s="151"/>
-      <c r="G1" s="151"/>
-      <c r="H1" s="151"/>
-      <c r="I1" s="151"/>
-      <c r="J1" s="151"/>
-      <c r="K1" s="151"/>
-      <c r="L1" s="151"/>
-      <c r="M1" s="151"/>
-      <c r="N1" s="151"/>
+      <c r="B1" s="159"/>
+      <c r="C1" s="159"/>
+      <c r="D1" s="159"/>
+      <c r="E1" s="159"/>
+      <c r="F1" s="159"/>
+      <c r="G1" s="159"/>
+      <c r="H1" s="159"/>
+      <c r="I1" s="159"/>
+      <c r="J1" s="159"/>
+      <c r="K1" s="159"/>
+      <c r="L1" s="159"/>
+      <c r="M1" s="159"/>
+      <c r="N1" s="159"/>
     </row>
     <row r="2" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="157" t="s">
+      <c r="A3" s="165" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="157"/>
-      <c r="C3" s="157"/>
-      <c r="E3" s="157" t="s">
+      <c r="B3" s="165"/>
+      <c r="C3" s="165"/>
+      <c r="E3" s="165" t="s">
         <v>193</v>
       </c>
-      <c r="F3" s="157"/>
-      <c r="G3" s="157"/>
-      <c r="H3" s="157"/>
-      <c r="I3" s="157"/>
-      <c r="J3" s="157"/>
-      <c r="K3" s="157"/>
-      <c r="L3" s="157"/>
-      <c r="M3" s="157"/>
-      <c r="N3" s="157"/>
+      <c r="F3" s="165"/>
+      <c r="G3" s="165"/>
+      <c r="H3" s="165"/>
+      <c r="I3" s="165"/>
+      <c r="J3" s="165"/>
+      <c r="K3" s="165"/>
+      <c r="L3" s="165"/>
+      <c r="M3" s="165"/>
+      <c r="N3" s="165"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="101" t="s">
@@ -11428,25 +11428,25 @@
       <c r="C4" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="158" t="s">
+      <c r="E4" s="166" t="s">
         <v>195</v>
       </c>
-      <c r="F4" s="156" t="s">
+      <c r="F4" s="164" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="156"/>
-      <c r="H4" s="156" t="s">
+      <c r="G4" s="164"/>
+      <c r="H4" s="164" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="156"/>
-      <c r="J4" s="156" t="s">
+      <c r="I4" s="164"/>
+      <c r="J4" s="164" t="s">
         <v>40</v>
       </c>
-      <c r="K4" s="156"/>
-      <c r="L4" s="156" t="s">
+      <c r="K4" s="164"/>
+      <c r="L4" s="164" t="s">
         <v>41</v>
       </c>
-      <c r="M4" s="156"/>
+      <c r="M4" s="164"/>
       <c r="N4" s="103"/>
     </row>
     <row r="5" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
@@ -11459,23 +11459,23 @@
       <c r="C5" s="38" t="s">
         <v>196</v>
       </c>
-      <c r="E5" s="158"/>
-      <c r="F5" s="156" t="s">
+      <c r="E5" s="166"/>
+      <c r="F5" s="164" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="156"/>
-      <c r="H5" s="156" t="s">
+      <c r="G5" s="164"/>
+      <c r="H5" s="164" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="156"/>
-      <c r="J5" s="156" t="s">
+      <c r="I5" s="164"/>
+      <c r="J5" s="164" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="156"/>
-      <c r="L5" s="156" t="s">
+      <c r="K5" s="164"/>
+      <c r="L5" s="164" t="s">
         <v>17</v>
       </c>
-      <c r="M5" s="156"/>
+      <c r="M5" s="164"/>
       <c r="N5" s="41" t="s">
         <v>197</v>
       </c>
@@ -11491,7 +11491,7 @@
       <c r="C6" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="158"/>
+      <c r="E6" s="166"/>
       <c r="F6" s="106">
         <f>B6*G6</f>
         <v>8.6450000000000014</v>
@@ -11923,11 +11923,11 @@
       <c r="N15" s="113"/>
     </row>
     <row r="16" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="157" t="s">
+      <c r="A16" s="165" t="s">
         <v>66</v>
       </c>
-      <c r="B16" s="157"/>
-      <c r="C16" s="157"/>
+      <c r="B16" s="165"/>
+      <c r="C16" s="165"/>
       <c r="E16" s="41" t="s">
         <v>217</v>
       </c>

</xml_diff>